<commit_message>
sauvegardee rapidee d'un truc qui predict mal mais qui lee fait eet c'est deja ca
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -667,7 +667,7 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="AC16" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="AC18" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="AC21" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="AC22" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="AC23" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Butterfly</t>
         </is>
       </c>
     </row>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="AC24" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Butterfly</t>
         </is>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="AC26" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="AC27" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="AC28" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="AC29" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3215,7 +3215,7 @@
       </c>
       <c r="AC30" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="AC31" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="AC32" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="AC33" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="AC34" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="AC35" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Butterfly</t>
         </is>
       </c>
     </row>
@@ -3761,7 +3761,7 @@
       </c>
       <c r="AC36" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="AC37" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Butterfly</t>
         </is>
       </c>
     </row>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="AC38" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="AC40" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Butterfly</t>
         </is>
       </c>
     </row>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="AC41" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="AC45" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Butterfly</t>
         </is>
       </c>
     </row>
@@ -4671,7 +4671,7 @@
       </c>
       <c r="AC46" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Butterfly</t>
         </is>
       </c>
     </row>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="AC48" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -4944,7 +4944,7 @@
       </c>
       <c r="AC49" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="AC51" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="AC52" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -5308,7 +5308,7 @@
       </c>
       <c r="AC53" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -5399,7 +5399,7 @@
       </c>
       <c r="AC54" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="AC56" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -5763,7 +5763,7 @@
       </c>
       <c r="AC58" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -5854,7 +5854,7 @@
       </c>
       <c r="AC59" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -5945,7 +5945,7 @@
       </c>
       <c r="AC60" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -6036,7 +6036,7 @@
       </c>
       <c r="AC61" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="AC63" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -6309,7 +6309,7 @@
       </c>
       <c r="AC64" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -6400,7 +6400,7 @@
       </c>
       <c r="AC65" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -6582,7 +6582,7 @@
       </c>
       <c r="AC67" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -6673,7 +6673,7 @@
       </c>
       <c r="AC68" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -6764,7 +6764,7 @@
       </c>
       <c r="AC69" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -6855,7 +6855,7 @@
       </c>
       <c r="AC70" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="AC74" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -7310,7 +7310,7 @@
       </c>
       <c r="AC75" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -7583,7 +7583,7 @@
       </c>
       <c r="AC78" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="AC79" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Butterfly</t>
         </is>
       </c>
     </row>
@@ -7765,7 +7765,7 @@
       </c>
       <c r="AC80" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -7947,7 +7947,7 @@
       </c>
       <c r="AC82" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -8038,7 +8038,7 @@
       </c>
       <c r="AC83" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -8220,7 +8220,7 @@
       </c>
       <c r="AC85" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -8311,7 +8311,7 @@
       </c>
       <c r="AC86" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -8402,7 +8402,7 @@
       </c>
       <c r="AC87" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -8493,7 +8493,7 @@
       </c>
       <c r="AC88" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -8584,7 +8584,7 @@
       </c>
       <c r="AC89" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -8857,7 +8857,7 @@
       </c>
       <c r="AC92" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -8948,7 +8948,7 @@
       </c>
       <c r="AC93" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -9039,7 +9039,7 @@
       </c>
       <c r="AC94" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -9130,7 +9130,7 @@
       </c>
       <c r="AC95" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="AC96" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -9312,7 +9312,7 @@
       </c>
       <c r="AC97" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>
@@ -9403,7 +9403,7 @@
       </c>
       <c r="AC98" t="inlineStr">
         <is>
-          <t>Bumblebee</t>
+          <t>Bee</t>
         </is>
       </c>
     </row>

</xml_diff>